<commit_message>
Payroll Computation, null date hired fix
</commit_message>
<xml_diff>
--- a/WebTemplate/Resources/Template/Payslip.xlsx
+++ b/WebTemplate/Resources/Template/Payslip.xlsx
@@ -893,7 +893,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,8 +1232,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A31" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -1916,7 +1916,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78" right="0.55000000000000004" top="0.12" bottom="0.2" header="0.5" footer="0.21"/>
-  <pageSetup scale="97" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="96" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Payroll Computation for outer port auto sunday and holiday, Personnel Loan new process
</commit_message>
<xml_diff>
--- a/WebTemplate/Resources/Template/Payslip.xlsx
+++ b/WebTemplate/Resources/Template/Payslip.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Trans-Pacific Journey Fishing Corporation</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Allowance</t>
-  </si>
-  <si>
-    <t>Night Differential:</t>
   </si>
   <si>
     <t xml:space="preserve">Deductions </t>
@@ -549,7 +546,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -823,6 +820,9 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -893,7 +893,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-1C00-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,8 +1232,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A31" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A19" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -1629,26 +1629,24 @@
     <row r="38" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A38" s="31"/>
       <c r="B38" s="32"/>
-      <c r="C38" s="29" t="s">
-        <v>27</v>
+      <c r="C38" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="D38" s="78"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="70"/>
+      <c r="F38" s="53"/>
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
       <c r="A39" s="31"/>
       <c r="B39" s="32"/>
-      <c r="C39" s="33" t="s">
-        <v>22</v>
-      </c>
+      <c r="C39" s="33"/>
       <c r="D39" s="39"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="53"/>
+      <c r="F39" s="98"/>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
       <c r="A40" s="95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="96"/>
       <c r="C40" s="96"/>
@@ -1658,14 +1656,14 @@
     </row>
     <row r="41" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A41" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="79">
         <v>0</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41" s="76">
         <v>0</v>
@@ -1674,14 +1672,14 @@
     </row>
     <row r="42" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A42" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="79">
         <v>0</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42" s="76">
         <v>0</v>
@@ -1690,14 +1688,14 @@
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A43" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" s="79">
         <v>0</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E43" s="76">
         <v>0</v>
@@ -1706,14 +1704,14 @@
     </row>
     <row r="44" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A44" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" s="79">
         <v>0</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="76">
         <v>0</v>
@@ -1723,7 +1721,7 @@
     </row>
     <row r="45" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
       <c r="A45" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" s="79">
         <v>0</v>
@@ -1736,7 +1734,7 @@
       <c r="B46" s="17"/>
       <c r="C46" s="42"/>
       <c r="D46" s="87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E46" s="87"/>
       <c r="F46" s="43"/>
@@ -1746,7 +1744,7 @@
       <c r="B47" s="84"/>
       <c r="C47" s="71"/>
       <c r="D47" s="72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E47" s="73"/>
       <c r="F47" s="74"/>
@@ -1764,7 +1762,7 @@
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
       <c r="D49" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="46"/>
@@ -1774,7 +1772,7 @@
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
       <c r="D50" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50" s="86"/>
       <c r="F50" s="86"/>
@@ -1785,7 +1783,7 @@
       <c r="C51" s="32"/>
       <c r="D51" s="32"/>
       <c r="E51" s="85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F51" s="85"/>
     </row>

</xml_diff>